<commit_message>
[Document, Modified] : Bảng yêu cầu nghiệp vụ
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/BangYeuCau_TrachNhiem/Bảng yêu cầu nghiệp vụ/Bảng yêu cầu nghiệp vụ.xlsx
+++ b/ToDoApp-Doc/Document/BangYeuCau_TrachNhiem/Bảng yêu cầu nghiệp vụ/Bảng yêu cầu nghiệp vụ.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="107">
   <si>
     <t>Danh sách các yêu cầu nghiệp vụ</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">                                                                                               Management Task
 BM4:
                                                                                               Form Update Task 
@@ -208,6 +214,13 @@
  Phân loại: 
 QĐ4: Tên task không được trùng. Mức độ ưu tiên từ 0-4.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                Management Subtask
+BM5:
+                                                                                          Form Create/Update Subtask
+Tên Subtask:
+QĐ5: Tên subtask không được trùng</t>
   </si>
   <si>
     <t xml:space="preserve">                                                                                                        Reminder
@@ -251,6 +264,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">                                                                                                          Repeater
 BM11:
                                                                                                     Form Repeater
@@ -386,6 +405,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">                                                                                                Manage User Notifications
 BM15:
                                                                                          Form Manage User Notifications
@@ -596,10 +621,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -639,6 +664,43 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -647,9 +709,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -657,7 +740,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -679,23 +778,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -711,42 +794,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -755,29 +802,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -804,13 +829,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -822,7 +847,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -834,7 +895,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -846,19 +937,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -876,37 +967,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -918,55 +979,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -978,13 +1009,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1050,11 +1075,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1076,11 +1107,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1102,24 +1146,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1132,27 +1172,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1170,134 +1195,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1331,6 +1356,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1433,7 +1459,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>838200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="7620000" cy="1114425"/>
@@ -1450,7 +1476,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1714500" y="29171900"/>
+          <a:off x="1714500" y="30887035"/>
           <a:ext cx="7620000" cy="1114425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1722,10 +1748,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z1041"/>
+  <dimension ref="A1:Z1043"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1"/>
@@ -2751,13 +2777,13 @@
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
     </row>
-    <row r="32" s="1" customFormat="1" ht="18.75" spans="1:26">
+    <row r="32" s="1" customFormat="1" ht="18.05" customHeight="1" spans="1:26">
       <c r="A32" s="2"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -2779,7 +2805,7 @@
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
     </row>
-    <row r="33" s="1" customFormat="1" ht="161" customHeight="1" spans="1:26">
+    <row r="33" s="1" customFormat="1" ht="117" customHeight="1" spans="1:26">
       <c r="A33" s="2"/>
       <c r="B33" s="9" t="s">
         <v>52</v>
@@ -2837,7 +2863,7 @@
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
     </row>
-    <row r="35" s="1" customFormat="1" ht="105" customHeight="1" spans="1:26">
+    <row r="35" s="1" customFormat="1" ht="161" customHeight="1" spans="1:26">
       <c r="A35" s="2"/>
       <c r="B35" s="9" t="s">
         <v>53</v>
@@ -2895,7 +2921,7 @@
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
     </row>
-    <row r="37" s="1" customFormat="1" ht="162" customHeight="1" spans="1:26">
+    <row r="37" s="1" customFormat="1" ht="105" customHeight="1" spans="1:26">
       <c r="A37" s="2"/>
       <c r="B37" s="9" t="s">
         <v>54</v>
@@ -2953,7 +2979,7 @@
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
     </row>
-    <row r="39" s="1" customFormat="1" ht="124" customHeight="1" spans="1:26">
+    <row r="39" s="1" customFormat="1" ht="162" customHeight="1" spans="1:26">
       <c r="A39" s="2"/>
       <c r="B39" s="9" t="s">
         <v>55</v>
@@ -3011,7 +3037,7 @@
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
     </row>
-    <row r="41" s="1" customFormat="1" ht="138" customHeight="1" spans="1:26">
+    <row r="41" s="1" customFormat="1" ht="124" customHeight="1" spans="1:26">
       <c r="A41" s="2"/>
       <c r="B41" s="9" t="s">
         <v>56</v>
@@ -3069,7 +3095,7 @@
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
     </row>
-    <row r="43" s="1" customFormat="1" ht="203" customHeight="1" spans="1:26">
+    <row r="43" s="1" customFormat="1" ht="138" customHeight="1" spans="1:26">
       <c r="A43" s="2"/>
       <c r="B43" s="9" t="s">
         <v>57</v>
@@ -3127,7 +3153,7 @@
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
     </row>
-    <row r="45" s="1" customFormat="1" ht="193" customHeight="1" spans="1:26">
+    <row r="45" s="1" customFormat="1" ht="203" customHeight="1" spans="1:26">
       <c r="A45" s="2"/>
       <c r="B45" s="9" t="s">
         <v>58</v>
@@ -3185,7 +3211,7 @@
       <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
     </row>
-    <row r="47" s="1" customFormat="1" ht="311" customHeight="1" spans="1:26">
+    <row r="47" s="1" customFormat="1" ht="193" customHeight="1" spans="1:26">
       <c r="A47" s="2"/>
       <c r="B47" s="9" t="s">
         <v>59</v>
@@ -3217,11 +3243,11 @@
     </row>
     <row r="48" s="1" customFormat="1" ht="18.75" spans="1:26">
       <c r="A48" s="2"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -3243,7 +3269,7 @@
       <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
     </row>
-    <row r="49" s="1" customFormat="1" ht="158" customHeight="1" spans="1:26">
+    <row r="49" s="1" customFormat="1" ht="311" customHeight="1" spans="1:26">
       <c r="A49" s="2"/>
       <c r="B49" s="9" t="s">
         <v>60</v>
@@ -3301,7 +3327,7 @@
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
     </row>
-    <row r="51" s="1" customFormat="1" ht="219" customHeight="1" spans="1:26">
+    <row r="51" s="1" customFormat="1" ht="158" customHeight="1" spans="1:26">
       <c r="A51" s="2"/>
       <c r="B51" s="9" t="s">
         <v>61</v>
@@ -3359,15 +3385,15 @@
       <c r="Y52" s="2"/>
       <c r="Z52" s="2"/>
     </row>
-    <row r="53" s="1" customFormat="1" ht="18.75" spans="1:26">
+    <row r="53" s="1" customFormat="1" ht="219" customHeight="1" spans="1:26">
       <c r="A53" s="2"/>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="11"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
@@ -3391,21 +3417,11 @@
     </row>
     <row r="54" s="1" customFormat="1" ht="18.75" spans="1:26">
       <c r="A54" s="2"/>
-      <c r="B54" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -3427,21 +3443,15 @@
       <c r="Y54" s="2"/>
       <c r="Z54" s="2"/>
     </row>
-    <row r="55" s="1" customFormat="1" ht="75" spans="1:26">
+    <row r="55" s="1" customFormat="1" ht="18.75" spans="1:26">
       <c r="A55" s="2"/>
-      <c r="B55" s="5">
-        <v>1</v>
+      <c r="B55" s="8" t="s">
+        <v>63</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F55" s="5"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
@@ -3463,21 +3473,23 @@
       <c r="Y55" s="2"/>
       <c r="Z55" s="2"/>
     </row>
-    <row r="56" s="1" customFormat="1" ht="75" spans="1:26">
+    <row r="56" s="1" customFormat="1" ht="18.75" spans="1:26">
       <c r="A56" s="2"/>
-      <c r="B56" s="5">
-        <v>2</v>
+      <c r="B56" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
-      <c r="F56" s="5"/>
+      <c r="F56" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
@@ -3499,19 +3511,19 @@
       <c r="Y56" s="2"/>
       <c r="Z56" s="2"/>
     </row>
-    <row r="57" s="1" customFormat="1" ht="56.25" spans="1:26">
+    <row r="57" s="1" customFormat="1" ht="75" spans="1:26">
       <c r="A57" s="2"/>
       <c r="B57" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="2"/>
@@ -3538,16 +3550,16 @@
     <row r="58" s="1" customFormat="1" ht="75" spans="1:26">
       <c r="A58" s="2"/>
       <c r="B58" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F58" s="5"/>
       <c r="G58" s="2"/>
@@ -3571,19 +3583,19 @@
       <c r="Y58" s="2"/>
       <c r="Z58" s="2"/>
     </row>
-    <row r="59" s="1" customFormat="1" ht="168.75" spans="1:26">
+    <row r="59" s="1" customFormat="1" ht="56.25" spans="1:26">
       <c r="A59" s="2"/>
       <c r="B59" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
-      <c r="D59" s="13" t="s">
-        <v>74</v>
+      <c r="D59" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="2"/>
@@ -3607,19 +3619,19 @@
       <c r="Y59" s="2"/>
       <c r="Z59" s="2"/>
     </row>
-    <row r="60" s="1" customFormat="1" ht="56.25" spans="1:26">
+    <row r="60" s="1" customFormat="1" ht="75" spans="1:26">
       <c r="A60" s="2"/>
       <c r="B60" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="2"/>
@@ -3643,19 +3655,19 @@
       <c r="Y60" s="2"/>
       <c r="Z60" s="2"/>
     </row>
-    <row r="61" s="1" customFormat="1" ht="91.5" customHeight="1" spans="1:26">
+    <row r="61" s="1" customFormat="1" ht="168.75" spans="1:26">
       <c r="A61" s="2"/>
       <c r="B61" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>78</v>
+      <c r="D61" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="2"/>
@@ -3679,19 +3691,19 @@
       <c r="Y61" s="2"/>
       <c r="Z61" s="2"/>
     </row>
-    <row r="62" s="1" customFormat="1" ht="85.5" customHeight="1" spans="1:26">
+    <row r="62" s="1" customFormat="1" ht="56.25" spans="1:26">
       <c r="A62" s="2"/>
       <c r="B62" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="2"/>
@@ -3715,19 +3727,19 @@
       <c r="Y62" s="2"/>
       <c r="Z62" s="2"/>
     </row>
-    <row r="63" s="1" customFormat="1" ht="76.5" customHeight="1" spans="1:26">
+    <row r="63" s="1" customFormat="1" ht="91.5" customHeight="1" spans="1:26">
       <c r="A63" s="2"/>
       <c r="B63" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F63" s="5"/>
       <c r="G63" s="2"/>
@@ -3751,19 +3763,19 @@
       <c r="Y63" s="2"/>
       <c r="Z63" s="2"/>
     </row>
-    <row r="64" s="1" customFormat="1" ht="37.5" spans="1:26">
+    <row r="64" s="1" customFormat="1" ht="85.5" customHeight="1" spans="1:26">
       <c r="A64" s="2"/>
       <c r="B64" s="5">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="2"/>
@@ -3787,19 +3799,19 @@
       <c r="Y64" s="2"/>
       <c r="Z64" s="2"/>
     </row>
-    <row r="65" s="1" customFormat="1" ht="75" spans="1:26">
+    <row r="65" s="1" customFormat="1" ht="76.5" customHeight="1" spans="1:26">
       <c r="A65" s="2"/>
       <c r="B65" s="5">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F65" s="5"/>
       <c r="G65" s="2"/>
@@ -3823,19 +3835,19 @@
       <c r="Y65" s="2"/>
       <c r="Z65" s="2"/>
     </row>
-    <row r="66" s="1" customFormat="1" ht="75" spans="1:26">
+    <row r="66" s="1" customFormat="1" ht="37.5" spans="1:26">
       <c r="A66" s="2"/>
       <c r="B66" s="5">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F66" s="5"/>
       <c r="G66" s="2"/>
@@ -3859,19 +3871,19 @@
       <c r="Y66" s="2"/>
       <c r="Z66" s="2"/>
     </row>
-    <row r="67" s="1" customFormat="1" ht="56.25" spans="1:26">
+    <row r="67" s="1" customFormat="1" ht="75" spans="1:26">
       <c r="A67" s="2"/>
       <c r="B67" s="5">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F67" s="5"/>
       <c r="G67" s="2"/>
@@ -3895,19 +3907,19 @@
       <c r="Y67" s="2"/>
       <c r="Z67" s="2"/>
     </row>
-    <row r="68" s="1" customFormat="1" ht="37.5" spans="1:26">
+    <row r="68" s="1" customFormat="1" ht="75" spans="1:26">
       <c r="A68" s="2"/>
       <c r="B68" s="5">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="2"/>
@@ -3934,16 +3946,16 @@
     <row r="69" s="1" customFormat="1" ht="56.25" spans="1:26">
       <c r="A69" s="2"/>
       <c r="B69" s="5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F69" s="5"/>
       <c r="G69" s="2"/>
@@ -3967,19 +3979,19 @@
       <c r="Y69" s="2"/>
       <c r="Z69" s="2"/>
     </row>
-    <row r="70" s="1" customFormat="1" ht="56.25" spans="1:26">
+    <row r="70" s="1" customFormat="1" ht="37.5" spans="1:26">
       <c r="A70" s="2"/>
       <c r="B70" s="5">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F70" s="5"/>
       <c r="G70" s="2"/>
@@ -4003,19 +4015,19 @@
       <c r="Y70" s="2"/>
       <c r="Z70" s="2"/>
     </row>
-    <row r="71" s="1" customFormat="1" ht="75" spans="1:26">
+    <row r="71" s="1" customFormat="1" ht="56.25" spans="1:26">
       <c r="A71" s="2"/>
       <c r="B71" s="5">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F71" s="5"/>
       <c r="G71" s="2"/>
@@ -4042,16 +4054,16 @@
     <row r="72" s="1" customFormat="1" ht="56.25" spans="1:26">
       <c r="A72" s="2"/>
       <c r="B72" s="5">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F72" s="5"/>
       <c r="G72" s="2"/>
@@ -4075,19 +4087,19 @@
       <c r="Y72" s="2"/>
       <c r="Z72" s="2"/>
     </row>
-    <row r="73" s="1" customFormat="1" ht="56.25" spans="1:26">
+    <row r="73" s="1" customFormat="1" ht="75" spans="1:26">
       <c r="A73" s="2"/>
       <c r="B73" s="5">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F73" s="5"/>
       <c r="G73" s="2"/>
@@ -4111,19 +4123,19 @@
       <c r="Y73" s="2"/>
       <c r="Z73" s="2"/>
     </row>
-    <row r="74" s="1" customFormat="1" ht="37.5" spans="1:26">
+    <row r="74" s="1" customFormat="1" ht="56.25" spans="1:26">
       <c r="A74" s="2"/>
       <c r="B74" s="5">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F74" s="5"/>
       <c r="G74" s="2"/>
@@ -4147,13 +4159,21 @@
       <c r="Y74" s="2"/>
       <c r="Z74" s="2"/>
     </row>
-    <row r="75" s="1" customFormat="1" ht="18" spans="1:26">
+    <row r="75" s="1" customFormat="1" ht="56.25" spans="1:26">
       <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
+      <c r="B75" s="5">
+        <v>19</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F75" s="5"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
@@ -4175,13 +4195,21 @@
       <c r="Y75" s="2"/>
       <c r="Z75" s="2"/>
     </row>
-    <row r="76" s="1" customFormat="1" ht="18" spans="1:26">
+    <row r="76" s="1" customFormat="1" ht="37.5" spans="1:26">
       <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
+      <c r="B76" s="5">
+        <v>20</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F76" s="5"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -31223,8 +31251,64 @@
       <c r="Y1041" s="2"/>
       <c r="Z1041" s="2"/>
     </row>
+    <row r="1042" s="1" customFormat="1" ht="18" spans="1:26">
+      <c r="A1042" s="2"/>
+      <c r="B1042" s="2"/>
+      <c r="C1042" s="2"/>
+      <c r="D1042" s="2"/>
+      <c r="E1042" s="2"/>
+      <c r="F1042" s="2"/>
+      <c r="G1042" s="2"/>
+      <c r="H1042" s="2"/>
+      <c r="I1042" s="2"/>
+      <c r="J1042" s="2"/>
+      <c r="K1042" s="2"/>
+      <c r="L1042" s="2"/>
+      <c r="M1042" s="2"/>
+      <c r="N1042" s="2"/>
+      <c r="O1042" s="2"/>
+      <c r="P1042" s="2"/>
+      <c r="Q1042" s="2"/>
+      <c r="R1042" s="2"/>
+      <c r="S1042" s="2"/>
+      <c r="T1042" s="2"/>
+      <c r="U1042" s="2"/>
+      <c r="V1042" s="2"/>
+      <c r="W1042" s="2"/>
+      <c r="X1042" s="2"/>
+      <c r="Y1042" s="2"/>
+      <c r="Z1042" s="2"/>
+    </row>
+    <row r="1043" s="1" customFormat="1" ht="18" spans="1:26">
+      <c r="A1043" s="2"/>
+      <c r="B1043" s="2"/>
+      <c r="C1043" s="2"/>
+      <c r="D1043" s="2"/>
+      <c r="E1043" s="2"/>
+      <c r="F1043" s="2"/>
+      <c r="G1043" s="2"/>
+      <c r="H1043" s="2"/>
+      <c r="I1043" s="2"/>
+      <c r="J1043" s="2"/>
+      <c r="K1043" s="2"/>
+      <c r="L1043" s="2"/>
+      <c r="M1043" s="2"/>
+      <c r="N1043" s="2"/>
+      <c r="O1043" s="2"/>
+      <c r="P1043" s="2"/>
+      <c r="Q1043" s="2"/>
+      <c r="R1043" s="2"/>
+      <c r="S1043" s="2"/>
+      <c r="T1043" s="2"/>
+      <c r="U1043" s="2"/>
+      <c r="V1043" s="2"/>
+      <c r="W1043" s="2"/>
+      <c r="X1043" s="2"/>
+      <c r="Y1043" s="2"/>
+      <c r="Z1043" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="B27:F27"/>
@@ -31241,6 +31325,7 @@
     <mergeCell ref="B49:F49"/>
     <mergeCell ref="B51:F51"/>
     <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B55:F55"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>